<commit_message>
Iniciando desafio robô registro identidade
</commit_message>
<xml_diff>
--- a/Robo_Extrator/ID/Identidades/Registro.xlsx
+++ b/Robo_Extrator/ID/Identidades/Registro.xlsx
@@ -498,9 +498,20 @@
         <x:v>123956789</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C2" s="2">
+        <x:v>31569</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:3">
+      <x:c r="A3" s="0" t="n">
+        <x:v>123956789</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="C2" s="2">
+      <x:c r="C3" s="2">
         <x:v>31569</x:v>
       </x:c>
     </x:row>

</xml_diff>